<commit_message>
Modificando el archivo gato en el master
</commit_message>
<xml_diff>
--- a/TAREA_GRUPO5/gato.xlsx
+++ b/TAREA_GRUPO5/gato.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roxan_000\Downloads\Autoevaluaci-n\TAREA_GRUPO5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA66A3A-AC39-43F5-AFDB-C39DE18FCE95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A217DB3-0FF0-4946-A382-B5151DE43395}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4335" yWindow="4290" windowWidth="14640" windowHeight="10290" xr2:uid="{E7FBD320-855E-446F-86B2-B31122A8189F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Tt = b0 + b1*t + b2*t^2 + b3*t^3</t>
   </si>
@@ -73,13 +73,43 @@
   </si>
   <si>
     <t>N =</t>
+  </si>
+  <si>
+    <t>z11</t>
+  </si>
+  <si>
+    <t>z12</t>
+  </si>
+  <si>
+    <t>z13</t>
+  </si>
+  <si>
+    <t>z14</t>
+  </si>
+  <si>
+    <t>z15</t>
+  </si>
+  <si>
+    <t>z16</t>
+  </si>
+  <si>
+    <t>z17</t>
+  </si>
+  <si>
+    <t>z18</t>
+  </si>
+  <si>
+    <t>z19</t>
+  </si>
+  <si>
+    <t>z20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +129,12 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -130,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -140,6 +176,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -455,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7518F89-64FF-40F8-99DC-D962B6AB64DE}">
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -640,9 +679,6 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
@@ -656,12 +692,176 @@
       <c r="E14" s="1">
         <f t="shared" si="1"/>
         <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1">
+        <v>11</v>
+      </c>
+      <c r="D15" s="1">
+        <f>C15^2</f>
+        <v>121</v>
+      </c>
+      <c r="E15" s="1">
+        <f>C15^3</f>
+        <v>1331</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="1">
+        <v>12</v>
+      </c>
+      <c r="D16" s="1">
+        <f t="shared" ref="D16:D23" si="2">C16^2</f>
+        <v>144</v>
+      </c>
+      <c r="E16" s="1">
+        <f t="shared" ref="E16:E23" si="3">C16^3</f>
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="1">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1">
+        <f t="shared" si="2"/>
+        <v>169</v>
+      </c>
+      <c r="E17" s="1">
+        <f t="shared" si="3"/>
+        <v>2197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1">
+        <v>14</v>
+      </c>
+      <c r="D18" s="1">
+        <f t="shared" si="2"/>
+        <v>196</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="3"/>
+        <v>2744</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1">
+        <v>15</v>
+      </c>
+      <c r="D19" s="1">
+        <f t="shared" si="2"/>
+        <v>225</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="3"/>
+        <v>3375</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="1">
+        <v>16</v>
+      </c>
+      <c r="D20" s="1">
+        <f t="shared" si="2"/>
+        <v>256</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="3"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="2"/>
+        <v>289</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="3"/>
+        <v>4913</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="1">
+        <v>18</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="2"/>
+        <v>324</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="3"/>
+        <v>5832</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="1">
+        <v>19</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="2"/>
+        <v>361</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="3"/>
+        <v>6859</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="1">
+        <v>20</v>
+      </c>
+      <c r="D24" s="1">
+        <f>C24^2</f>
+        <v>400</v>
+      </c>
+      <c r="E24" s="1">
+        <f>C24^3</f>
+        <v>8000</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>